<commit_message>
Update test_sequences files with headers
</commit_message>
<xml_diff>
--- a/tests/test_sequences/simple.headers.xlsx
+++ b/tests/test_sequences/simple.headers.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>seqid</t>
+  </si>
+  <si>
+    <t>voucher</t>
   </si>
   <si>
     <t>sequences</t>
@@ -22,16 +25,25 @@
     <t>id1</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>ATC</t>
   </si>
   <si>
     <t>id2</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>ATG</t>
   </si>
   <si>
     <t>id3</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
   <si>
     <t>ATA</t>
@@ -93,7 +105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -136,7 +148,7 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
@@ -148,7 +160,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -164,6 +176,36 @@
     <border>
       <left style="thin">
         <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -212,7 +254,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -231,22 +273,28 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1349,7 +1397,9 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -1357,204 +1407,210 @@
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="C2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B3" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C3" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>